<commit_message>
Change in submission ecel
</commit_message>
<xml_diff>
--- a/Submission_list_Java.xlsx
+++ b/Submission_list_Java.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,12 +438,12 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1">
+    <row r="2" spans="1:4" ht="16.2" thickBot="1">
       <c r="A2" s="2">
         <v>501</v>
       </c>
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1">
+    <row r="3" spans="1:4" ht="16.2" thickBot="1">
       <c r="A3" s="2">
         <v>502</v>
       </c>
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1">
+    <row r="4" spans="1:4" ht="16.2" thickBot="1">
       <c r="A4" s="2">
         <v>503</v>
       </c>
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1">
+    <row r="5" spans="1:4" ht="16.2" thickBot="1">
       <c r="A5" s="2">
         <v>504</v>
       </c>
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1">
+    <row r="6" spans="1:4" ht="16.2" thickBot="1">
       <c r="A6" s="2">
         <v>506</v>
       </c>
@@ -524,10 +524,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.2" thickBot="1">
       <c r="A7" s="2">
         <v>509</v>
       </c>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1">
+    <row r="8" spans="1:4" ht="16.2" thickBot="1">
       <c r="A8" s="2">
         <v>510</v>
       </c>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" thickBot="1">
+    <row r="9" spans="1:4" ht="16.2" thickBot="1">
       <c r="A9" s="2">
         <v>513</v>
       </c>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16.5" thickBot="1">
+    <row r="10" spans="1:4" ht="16.2" thickBot="1">
       <c r="A10" s="2">
         <v>514</v>
       </c>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" thickBot="1">
+    <row r="11" spans="1:4" ht="16.2" thickBot="1">
       <c r="A11" s="2">
         <v>515</v>
       </c>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16.5" thickBot="1">
+    <row r="12" spans="1:4" ht="16.2" thickBot="1">
       <c r="A12" s="2">
         <v>516</v>
       </c>
@@ -611,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16.5" thickBot="1">
+    <row r="13" spans="1:4" ht="16.2" thickBot="1">
       <c r="A13" s="2">
         <v>517</v>
       </c>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16.5" thickBot="1">
+    <row r="14" spans="1:4" ht="16.2" thickBot="1">
       <c r="A14" s="2">
         <v>518</v>
       </c>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16.5" thickBot="1">
+    <row r="15" spans="1:4" ht="16.2" thickBot="1">
       <c r="A15" s="2">
         <v>519</v>
       </c>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16.5" thickBot="1">
+    <row r="16" spans="1:4" ht="16.2" thickBot="1">
       <c r="A16" s="2">
         <v>520</v>
       </c>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1">
+    <row r="17" spans="1:4" ht="16.2" thickBot="1">
       <c r="A17" s="2">
         <v>521</v>
       </c>
@@ -681,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16.5" thickBot="1">
+    <row r="18" spans="1:4" ht="16.2" thickBot="1">
       <c r="A18" s="2">
         <v>522</v>
       </c>
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16.5" thickBot="1">
+    <row r="19" spans="1:4" ht="16.2" thickBot="1">
       <c r="A19" s="2">
         <v>523</v>
       </c>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16.5" thickBot="1">
+    <row r="20" spans="1:4" ht="16.2" thickBot="1">
       <c r="A20" s="2">
         <v>524</v>
       </c>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16.5" thickBot="1">
+    <row r="21" spans="1:4" ht="16.2" thickBot="1">
       <c r="A21" s="2">
         <v>528</v>
       </c>
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16.5" thickBot="1">
+    <row r="22" spans="1:4" ht="16.2" thickBot="1">
       <c r="A22" s="2">
         <v>529</v>
       </c>
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16.5" thickBot="1">
+    <row r="23" spans="1:4" ht="16.2" thickBot="1">
       <c r="A23" s="2">
         <v>530</v>
       </c>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1">
+    <row r="24" spans="1:4" ht="16.2" thickBot="1">
       <c r="A24" s="5">
         <v>531</v>
       </c>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" thickBot="1">
+    <row r="25" spans="1:4" ht="16.2" thickBot="1">
       <c r="A25" s="5">
         <v>532</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" thickBot="1">
+    <row r="26" spans="1:4" ht="16.2" thickBot="1">
       <c r="A26" s="5">
         <v>533</v>
       </c>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1">
+    <row r="27" spans="1:4" ht="16.2" thickBot="1">
       <c r="A27" s="5">
         <v>535</v>
       </c>
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" thickBot="1">
+    <row r="28" spans="1:4" ht="16.2" thickBot="1">
       <c r="A28" s="5">
         <v>536</v>
       </c>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1">
+    <row r="29" spans="1:4" ht="16.2" thickBot="1">
       <c r="A29" s="5">
         <v>538</v>
       </c>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" thickBot="1">
+    <row r="30" spans="1:4" ht="16.2" thickBot="1">
       <c r="A30" s="5">
         <v>539</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5" thickBot="1">
+    <row r="31" spans="1:4" ht="16.2" thickBot="1">
       <c r="A31" s="5">
         <v>541</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16.5" thickBot="1">
+    <row r="32" spans="1:4" ht="16.2" thickBot="1">
       <c r="A32" s="5">
         <v>542</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.5" thickBot="1">
+    <row r="33" spans="1:4" ht="16.2" thickBot="1">
       <c r="A33" s="5">
         <v>543</v>
       </c>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16.5" thickBot="1">
+    <row r="34" spans="1:4" ht="16.2" thickBot="1">
       <c r="A34" s="5">
         <v>544</v>
       </c>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16.5" thickBot="1">
+    <row r="35" spans="1:4" ht="16.2" thickBot="1">
       <c r="A35" s="5">
         <v>545</v>
       </c>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16.5" thickBot="1">
+    <row r="36" spans="1:4" ht="16.2" thickBot="1">
       <c r="A36" s="5">
         <v>546</v>
       </c>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16.5" thickBot="1">
+    <row r="37" spans="1:4" ht="16.2" thickBot="1">
       <c r="A37" s="5">
         <v>548</v>
       </c>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16.5" thickBot="1">
+    <row r="38" spans="1:4" ht="16.2" thickBot="1">
       <c r="A38" s="5">
         <v>549</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16.5" thickBot="1">
+    <row r="39" spans="1:4" ht="16.2" thickBot="1">
       <c r="A39" s="5">
         <v>553</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16.5" thickBot="1">
+    <row r="40" spans="1:4" ht="16.2" thickBot="1">
       <c r="A40" s="6">
         <v>555</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16.5" thickBot="1">
+    <row r="41" spans="1:4" ht="16.2" thickBot="1">
       <c r="A41" s="6">
         <v>557</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16.5" thickBot="1">
+    <row r="42" spans="1:4" ht="16.2" thickBot="1">
       <c r="A42" s="6">
         <v>558</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16.5" thickBot="1">
+    <row r="43" spans="1:4" ht="16.2" thickBot="1">
       <c r="A43" s="5">
         <v>559</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.5" thickBot="1">
+    <row r="44" spans="1:4" ht="16.2" thickBot="1">
       <c r="A44" s="5">
         <v>561</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16.5" thickBot="1">
+    <row r="45" spans="1:4" ht="16.2" thickBot="1">
       <c r="A45" s="5">
         <v>563</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16.5" thickBot="1">
+    <row r="46" spans="1:4" ht="16.2" thickBot="1">
       <c r="A46" s="5">
         <v>564</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16.5" thickBot="1">
+    <row r="47" spans="1:4" ht="16.2" thickBot="1">
       <c r="A47" s="5">
         <v>566</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16.5" thickBot="1">
+    <row r="48" spans="1:4" ht="16.2" thickBot="1">
       <c r="A48" s="5">
         <v>567</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16.5" thickBot="1">
+    <row r="49" spans="1:4" ht="16.2" thickBot="1">
       <c r="A49" s="5">
         <v>568</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16.5" thickBot="1">
+    <row r="50" spans="1:4" ht="16.2" thickBot="1">
       <c r="A50" s="5">
         <v>571</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16.5" thickBot="1">
+    <row r="51" spans="1:4" ht="16.2" thickBot="1">
       <c r="A51" s="5">
         <v>573</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16.5" thickBot="1">
+    <row r="52" spans="1:4" ht="16.2" thickBot="1">
       <c r="A52" s="5">
         <v>574</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16.5" thickBot="1">
+    <row r="53" spans="1:4" ht="16.2" thickBot="1">
       <c r="A53" s="5">
         <v>575</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16.5" thickBot="1">
+    <row r="54" spans="1:4" ht="16.2" thickBot="1">
       <c r="A54" s="5">
         <v>576</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16.5" thickBot="1">
+    <row r="55" spans="1:4" ht="16.2" thickBot="1">
       <c r="A55" s="5">
         <v>581</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16.5" thickBot="1">
+    <row r="56" spans="1:4" ht="16.2" thickBot="1">
       <c r="A56" s="5">
         <v>582</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16.5" thickBot="1">
+    <row r="57" spans="1:4" ht="16.2" thickBot="1">
       <c r="A57" s="5">
         <v>584</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16.5" thickBot="1">
+    <row r="58" spans="1:4" ht="16.2" thickBot="1">
       <c r="A58" s="5">
         <v>586</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16.5" thickBot="1">
+    <row r="59" spans="1:4" ht="16.2" thickBot="1">
       <c r="A59" s="5">
         <v>587</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16.5" thickBot="1">
+    <row r="60" spans="1:4" ht="16.2" thickBot="1">
       <c r="A60" s="5">
         <v>588</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16.5" thickBot="1">
+    <row r="61" spans="1:4" ht="16.2" thickBot="1">
       <c r="A61" s="5">
         <v>590</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16.5" thickBot="1">
+    <row r="62" spans="1:4" ht="16.2" thickBot="1">
       <c r="A62" s="5">
         <v>592</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16.5" thickBot="1">
+    <row r="63" spans="1:4" ht="16.2" thickBot="1">
       <c r="A63" s="5">
         <v>594</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16.5" thickBot="1">
+    <row r="64" spans="1:4" ht="16.2" thickBot="1">
       <c r="A64" s="5">
         <v>595</v>
       </c>
@@ -1351,7 +1351,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1363,7 +1363,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>